<commit_message>
get component name for package
</commit_message>
<xml_diff>
--- a/adb/packages.xlsx
+++ b/adb/packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kushn\projects\adaptive-ui\android-adaptive-ui\adb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC864AD-082E-44B9-8633-62929CF05A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA426A68-180B-40AD-9951-0FD8E454E3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4C8A2E58-F25E-4BF3-AB9C-37425D1864C5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="1420">
   <si>
     <t>package:/system_ext/app/PersistentBackgroundCameraServices/PersistentBackgroundCameraServices.apk</t>
   </si>
@@ -4296,6 +4296,9 @@
   </si>
   <si>
     <t>clock</t>
+  </si>
+  <si>
+    <t>camera</t>
   </si>
 </sst>
 </file>
@@ -10155,8 +10158,8 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10426,6 +10429,9 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>935</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1419</v>
       </c>
       <c r="F25" t="s">
         <v>1277</v>

</xml_diff>